<commit_message>
Adjust on PLANO DE TESTE.xlsx e README.md
Signed-off-by: kauefelippet <kaue.andrea.elias@gmail.com>
</commit_message>
<xml_diff>
--- a/PLANO DE TESTE.xlsx
+++ b/PLANO DE TESTE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93ecdcdf8c11fe19/FACENS/4º Semestre/UI UX e Testes de Software/AF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\facens-white-box-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{713E859F-15A1-4F8D-96ED-859B57252448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F14171-4525-4316-B481-6893E8025D3C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0943914A-238C-4A9E-B9F3-19E5DB8BC494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="5220" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17895" yWindow="5340" windowWidth="18000" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAIXA BRANCA (ESTÁTICO)" sheetId="3" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>O código foi devidamente documentado?</t>
   </si>
   <si>
-    <t>Inserir comentários explicando o motivo das escolhas e implementações</t>
-  </si>
-  <si>
     <t>KAUÊ FELIPPE TIBURCIO</t>
   </si>
   <si>
@@ -86,13 +83,16 @@
     <t>O código não fecha Connection, Statement e ResultSet</t>
   </si>
   <si>
-    <t>Inserir close()</t>
-  </si>
-  <si>
     <t>Inserir validação de conn e tratamento de exceções</t>
   </si>
   <si>
-    <t>User.java - O código não possui nenhum comentário descritivo sobre seu funcionamento.</t>
+    <t>O código não possui nenhum comentário descritivo útil sobre seu funcionamento</t>
+  </si>
+  <si>
+    <t>Adicionar JavaDoc explicando parâmetros, retornos e exceções</t>
+  </si>
+  <si>
+    <t>Usar try-with-resources para fechar `Connection`, `PreparedStatement` e `ResultSet` automaticamente</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +701,7 @@
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -744,10 +744,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -755,7 +755,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>9</v>
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>9</v>
@@ -781,33 +781,33 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>